<commit_message>
Création du buffer MONO pour analyse (dans importation)
</commit_message>
<xml_diff>
--- a/Architecture/LFO_2022_Mosaique-noms_recurrents.xlsx
+++ b/Architecture/LFO_2022_Mosaique-noms_recurrents.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25428"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10708"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3B8B04F5-17EC-4414-8FEA-7FC41289A941}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F031FD8B-E1DB-CE4D-8B00-50325254B0F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28560" windowHeight="13545" xr2:uid="{087A1B5B-7B97-4327-AC94-7D0ECF997B43}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="28560" windowHeight="13540" xr2:uid="{087A1B5B-7B97-4327-AC94-7D0ECF997B43}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Listes des noms d'objets LFO 2022 - Mosaïque</t>
   </si>
@@ -111,13 +111,19 @@
   </si>
   <si>
     <t>pour garder en mémoire quels paramètres d'analyse ont été cochés</t>
+  </si>
+  <si>
+    <t>#1Mosaique_corpusAudioMONO</t>
+  </si>
+  <si>
+    <t>buffer audio mono pour l'analyse</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -166,9 +172,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Bureau">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -206,7 +212,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Bureau">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -312,7 +318,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Bureau">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -462,24 +468,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B7EDC20-7B7C-4A7E-972E-FECEFF2E9DC1}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="40.140625" customWidth="1"/>
+    <col min="1" max="1" width="40.1640625" customWidth="1"/>
     <col min="2" max="2" width="56" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -487,7 +493,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -495,7 +501,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -503,7 +509,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -511,75 +517,83 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>9</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>11</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>13</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>15</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>17</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>19</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
-      <c r="A13" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>21</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
-      <c r="A14" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>23</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
-      <c r="A15" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>25</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>